<commit_message>
chỉnh sửa để chọn cam mặc định luôn là 1
</commit_message>
<xml_diff>
--- a/reports/attendance_report_2025-05-31.xlsx
+++ b/reports/attendance_report_2025-05-31.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -490,7 +490,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>anhtonton</t>
+          <t>bellingham</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -517,7 +517,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>bellingham</t>
+          <t>benzema</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -544,7 +544,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>benzema</t>
+          <t>carvajal</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -571,7 +571,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>carvajal</t>
+          <t>courtois</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -598,7 +598,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>courtois</t>
+          <t>kevin</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -625,7 +625,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>kevin</t>
+          <t>mbappe</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -652,7 +652,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>mbappe</t>
+          <t>messi</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -679,7 +679,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>messi</t>
+          <t>modric</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -706,7 +706,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>modric</t>
+          <t>mtp</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -733,7 +733,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>mtp</t>
+          <t>neymar</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -760,7 +760,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>neymar</t>
+          <t>ronaldo</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -787,7 +787,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>ronaldo</t>
+          <t>vietANH</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -835,6 +835,60 @@
       <c r="E15" t="inlineStr">
         <is>
           <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>QA</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Có mặt</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>16:09:43</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Chưa checkout</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>anhtonton</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Có mặt</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>16:09:37</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Chưa checkout</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
tạo ứng dụng cho người dùng
</commit_message>
<xml_diff>
--- a/reports/attendance_report_2025-05-31.xlsx
+++ b/reports/attendance_report_2025-05-31.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -787,108 +787,27 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>vietANH</t>
+          <t>anhtonton</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Vắng mặt</t>
+          <t>Có mặt</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>20:59:19</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>20:59:24</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>vinicius</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Vắng mặt</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>QA</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Có mặt</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>16:09:43</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>Chưa checkout</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>anhtonton</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Có mặt</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>16:09:37</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>Chưa checkout</t>
+          <t>00:00:05</t>
         </is>
       </c>
     </row>

</xml_diff>